<commit_message>
Improve access to data TimeSeries, update data plotting
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_diabetes.xlsx
+++ b/tests/databooks/databook_diabetes.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DA645CF1-D858-364C-BC66-3CEEA98BF104}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B602519B-76A2-43A2-B363-97FE187F41E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="18560" windowHeight="13440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="18555" windowHeight="13440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Population Definitions" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="4" r:id="rId2"/>
     <sheet name="State Variables" sheetId="5" r:id="rId3"/>
-    <sheet name="Metadata" sheetId="6" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -1495,7 +1494,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="43">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -1588,15 +1587,6 @@
   </si>
   <si>
     <t>Proportion with HbA1c control</t>
-  </si>
-  <si>
-    <t>data_start</t>
-  </si>
-  <si>
-    <t>data_end</t>
-  </si>
-  <si>
-    <t>data_dt</t>
   </si>
   <si>
     <t>adults</t>
@@ -2073,12 +2063,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2086,12 +2076,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2105,18 +2095,18 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" style="5" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -2139,10 +2129,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -2159,7 +2149,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -2182,10 +2172,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -2202,7 +2192,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2225,10 +2215,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -2245,7 +2235,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -2268,10 +2258,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -2288,7 +2278,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -2311,10 +2301,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -2331,7 +2321,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -2354,10 +2344,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -2374,7 +2364,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -2397,10 +2387,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -2417,7 +2407,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -2440,10 +2430,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2460,7 +2450,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -2483,10 +2473,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2503,7 +2493,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2526,10 +2516,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -2546,7 +2536,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>18</v>
       </c>
@@ -2569,10 +2559,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -2589,7 +2579,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
@@ -2612,10 +2602,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -2632,7 +2622,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>20</v>
       </c>
@@ -2655,10 +2645,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B38" t="s">
         <v>17</v>
@@ -2696,21 +2686,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView zoomScale="139" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -2731,10 +2721,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -2751,9 +2741,9 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -2774,10 +2764,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -2794,9 +2784,9 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -2817,10 +2807,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -2837,9 +2827,9 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -2860,10 +2850,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -2880,9 +2870,9 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -2903,10 +2893,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -2923,9 +2913,9 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -2946,10 +2936,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -2966,9 +2956,9 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -2989,10 +2979,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -3009,9 +2999,9 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>3</v>
@@ -3032,10 +3022,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3052,9 +3042,9 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -3075,10 +3065,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -3095,9 +3085,9 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>3</v>
@@ -3118,10 +3108,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -3138,7 +3128,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>21</v>
       </c>
@@ -3161,10 +3151,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -3181,7 +3171,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>22</v>
       </c>
@@ -3204,10 +3194,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -3224,7 +3214,7 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>23</v>
       </c>
@@ -3247,10 +3237,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -3267,7 +3257,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>24</v>
       </c>
@@ -3290,10 +3280,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
@@ -3310,7 +3300,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>25</v>
       </c>
@@ -3333,10 +3323,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
@@ -3353,7 +3343,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>26</v>
       </c>
@@ -3376,10 +3366,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B47" t="s">
         <v>27</v>
@@ -3396,7 +3386,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>28</v>
       </c>
@@ -3419,10 +3409,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B50" t="s">
         <v>27</v>
@@ -3439,7 +3429,7 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>29</v>
       </c>
@@ -3462,10 +3452,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B53" t="s">
         <v>27</v>
@@ -3482,7 +3472,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>30</v>
       </c>
@@ -3505,10 +3495,10 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="str">
-        <f>'Population Definitions'!$B$2</f>
-        <v>Adults</v>
+        <f>'Population Definitions'!$A$2</f>
+        <v>adults</v>
       </c>
       <c r="B56" t="s">
         <v>27</v>
@@ -3537,41 +3527,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>